<commit_message>
Updated backlog and added rules
</commit_message>
<xml_diff>
--- a/backlog_project.xlsx
+++ b/backlog_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\project-groep_23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74507A2-0A54-4DAF-A3A6-209F2F6B8E37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B270B5A0-ED3E-4B3E-9BFC-632391445428}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17220" yWindow="5115" windowWidth="21600" windowHeight="11385" xr2:uid="{E7A0AC40-04B9-4F77-9D38-CCE5C3D4FB7D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E7A0AC40-04B9-4F77-9D38-CCE5C3D4FB7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>Task Description</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Bug fixes en tests</t>
+  </si>
+  <si>
+    <t>Verdediging voorbereiden</t>
   </si>
 </sst>
 </file>
@@ -1901,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40880F0-B5E8-4115-9C74-D48698FDE8C6}">
   <dimension ref="A1:AS36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2568,6 +2571,12 @@
       </c>
     </row>
     <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="B34" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>38</v>
+      </c>
       <c r="D34" s="14">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
added capitals  to the classes
</commit_message>
<xml_diff>
--- a/backlog_project.xlsx
+++ b/backlog_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project ogp1\project-groep_23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA56368-8EDB-4FA5-A530-B1EF5D189103}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C4C18B-6A66-43A6-B146-BB810156F05A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E7A0AC40-04B9-4F77-9D38-CCE5C3D4FB7D}"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="21600" windowHeight="11865" xr2:uid="{E7A0AC40-04B9-4F77-9D38-CCE5C3D4FB7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1898,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40880F0-B5E8-4115-9C74-D48698FDE8C6}">
   <dimension ref="A1:AS37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,7 +2254,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="13">
         <v>4</v>
@@ -2275,7 +2275,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="13">
         <v>3</v>

</xml_diff>

<commit_message>
added some needed functionality
</commit_message>
<xml_diff>
--- a/backlog_project.xlsx
+++ b/backlog_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\project-groep_23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project ogp1\project-groep_23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8048EECD-6FA1-4F8A-88C0-A6ED83E1DA3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FC0F12-354C-4EE2-B071-C8A0C17AFC5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E7A0AC40-04B9-4F77-9D38-CCE5C3D4FB7D}"/>
+    <workbookView xWindow="2835" yWindow="0" windowWidth="21600" windowHeight="11865" xr2:uid="{E7A0AC40-04B9-4F77-9D38-CCE5C3D4FB7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -312,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -357,9 +348,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -382,7 +376,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -645,7 +639,7 @@
                   <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1609,7 +1603,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1908,7 +1902,7 @@
   <dimension ref="A1:AS37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2386,6 +2380,9 @@
       <c r="I15" s="13">
         <v>2</v>
       </c>
+      <c r="J15" s="22">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:45" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
@@ -2926,7 +2923,7 @@
       </c>
       <c r="J37" s="13">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K37" s="13">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
added a widget to pay for buildings
</commit_message>
<xml_diff>
--- a/backlog_project.xlsx
+++ b/backlog_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project ogp1\project-groep_23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278D6643-8599-44FB-BF6C-9A43092DD26C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EAE24B-89C1-4429-BE21-667878AD95EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{E7A0AC40-04B9-4F77-9D38-CCE5C3D4FB7D}"/>
   </bookViews>
@@ -642,7 +642,7 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1899,7 +1899,7 @@
   <dimension ref="A1:AS37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3951,6 +3951,9 @@
       <c r="K27" s="13">
         <v>3</v>
       </c>
+      <c r="L27" s="13">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
@@ -3960,7 +3963,7 @@
         <v>11</v>
       </c>
       <c r="D28" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="13">
         <v>4</v>
@@ -3982,6 +3985,9 @@
       </c>
       <c r="K28" s="13">
         <v>3</v>
+      </c>
+      <c r="L28" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:45" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -4202,7 +4208,7 @@
       </c>
       <c r="D37" s="14">
         <f>SUM(D5:D35)/25</f>
-        <v>0.5</v>
+        <v>0.54</v>
       </c>
       <c r="E37" s="13">
         <f>SUM(E6:E36)</f>
@@ -4234,7 +4240,7 @@
       </c>
       <c r="L37" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M37" s="13">
         <f t="shared" si="1"/>

</xml_diff>